<commit_message>
CCR was missing the updated template for social impressions
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@5549 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/vendors/consolidated_report/templates/consolidated_report_revision-12.xlsx
+++ b/app/vendors/consolidated_report/templates/consolidated_report_revision-12.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\toolbox\development\app\vendors\consolidated_report\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Development\toolbox\app\vendors\consolidated_report\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4725" windowWidth="19440" windowHeight="5400" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="4725" windowWidth="19440" windowHeight="5400" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="4" state="hidden" r:id="rId1"/>
@@ -1786,11 +1786,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2005462432"/>
-        <c:axId val="2005458624"/>
+        <c:axId val="800948912"/>
+        <c:axId val="800944560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2005462432"/>
+        <c:axId val="800948912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1818,7 +1818,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2005458624"/>
+        <c:crossAx val="800944560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1826,7 +1826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2005458624"/>
+        <c:axId val="800944560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1854,7 +1854,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2005462432"/>
+        <c:crossAx val="800948912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2099,12 +2099,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="2005461344"/>
-        <c:axId val="2005460256"/>
+        <c:axId val="800729488"/>
+        <c:axId val="800725136"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2005461344"/>
+        <c:axId val="800729488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2132,7 +2132,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2005460256"/>
+        <c:crossAx val="800725136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2140,7 +2140,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2005460256"/>
+        <c:axId val="800725136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2168,7 +2168,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2005461344"/>
+        <c:crossAx val="800729488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2420,12 +2420,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="2005456448"/>
-        <c:axId val="2005456992"/>
+        <c:axId val="800728400"/>
+        <c:axId val="800722960"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2005456448"/>
+        <c:axId val="800728400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2453,7 +2453,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2005456992"/>
+        <c:crossAx val="800722960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2461,7 +2461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2005456992"/>
+        <c:axId val="800722960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2489,7 +2489,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2005456448"/>
+        <c:crossAx val="800728400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2716,12 +2716,12 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="2006326080"/>
-        <c:axId val="2006324448"/>
+        <c:axId val="800726224"/>
+        <c:axId val="800726768"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2006326080"/>
+        <c:axId val="800726224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2744,7 +2744,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2006324448"/>
+        <c:crossAx val="800726768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2752,7 +2752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2006324448"/>
+        <c:axId val="800726768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2763,7 +2763,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2006326080"/>
+        <c:crossAx val="800726224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4351,7 +4351,7 @@
   </sheetPr>
   <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScale="75" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7809,9 +7809,9 @@
     <hyperlink ref="I38" location="'Key - Legend'!A1" display="Please see legend for descriptions"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="74" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup scale="72" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;R&amp;9&amp;K003366Luxury Link Travel Group: Client Report  for May 2011</oddFooter>
+    <oddFooter>&amp;R&amp;9&amp;K003366Luxury Link Travel Group: Client Report</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -8480,11 +8480,11 @@
     <hyperlink ref="F31" location="'Key - Legend'!A1" display="Please see legend for descriptions"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="99" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;R&amp;9&amp;K003366Luxury Link Travel Group: Client Report  for May 2011</oddFooter>
+    <oddFooter>&amp;R&amp;9&amp;K003366Luxury Link Travel Group: Client Report</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9286,7 +9286,7 @@
         <v>0</v>
       </c>
       <c r="O23" s="56">
-        <f t="shared" ref="O22:O24" si="2">SUM(B23:M23)</f>
+        <f t="shared" ref="O23" si="2">SUM(B23:M23)</f>
         <v>0</v>
       </c>
       <c r="P23" s="25">
@@ -10123,9 +10123,9 @@
     <hyperlink ref="O33" location="'Key - Legend'!A1" display="Please see legend for descriptions"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="74" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup scale="62" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;R&amp;9&amp;K003366Luxury Link Travel Group: Client Report  for May 2011</oddFooter>
+    <oddFooter>&amp;R&amp;9&amp;K003366Luxury Link Travel Group: Client Report</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -48242,9 +48242,9 @@
     <hyperlink ref="M9" location="'Key - Legend'!A1" display="Opt-In"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="52" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup scale="55" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;R&amp;9&amp;K003366Luxury Link Travel Group: Client Report  for May 2011</oddFooter>
+    <oddFooter>&amp;R&amp;9&amp;K003366Luxury Link Travel Group: Client Report</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
@@ -48259,7 +48259,7 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -48459,7 +48459,7 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.40444444444444444" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="95" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup scale="96" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Report template should open to the dashboard tab
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@5554 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/vendors/consolidated_report/templates/consolidated_report_revision-12.xlsx
+++ b/app/vendors/consolidated_report/templates/consolidated_report_revision-12.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Development\toolbox\app\vendors\consolidated_report\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\toolbox\release\app\vendors\consolidated_report\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4725" windowWidth="19440" windowHeight="5400" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="4725" windowWidth="19440" windowHeight="5400" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="4" state="hidden" r:id="rId1"/>
@@ -1738,7 +1738,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -1786,11 +1785,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="800948912"/>
-        <c:axId val="800944560"/>
+        <c:axId val="1191278128"/>
+        <c:axId val="1317000560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="800948912"/>
+        <c:axId val="1191278128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1818,7 +1817,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="800944560"/>
+        <c:crossAx val="1317000560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1826,7 +1825,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="800944560"/>
+        <c:axId val="1317000560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1854,7 +1853,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="800948912"/>
+        <c:crossAx val="1191278128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1869,7 +1868,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
@@ -2099,12 +2097,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="800729488"/>
-        <c:axId val="800725136"/>
+        <c:axId val="1317000016"/>
+        <c:axId val="1317003824"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="800729488"/>
+        <c:axId val="1317000016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2132,7 +2130,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="800725136"/>
+        <c:crossAx val="1317003824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2140,7 +2138,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="800725136"/>
+        <c:axId val="1317003824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2168,7 +2166,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="800729488"/>
+        <c:crossAx val="1317000016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2245,7 +2243,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2420,12 +2417,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="800728400"/>
-        <c:axId val="800722960"/>
+        <c:axId val="1317002192"/>
+        <c:axId val="1316998928"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="800728400"/>
+        <c:axId val="1317002192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2453,7 +2450,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="800722960"/>
+        <c:crossAx val="1316998928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2461,7 +2458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="800722960"/>
+        <c:axId val="1316998928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2489,7 +2486,7 @@
             <a:prstDash val="solid"/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="800728400"/>
+        <c:crossAx val="1317002192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2572,7 +2569,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2671,7 +2667,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -2716,12 +2711,12 @@
         </c:dLbls>
         <c:gapWidth val="95"/>
         <c:shape val="box"/>
-        <c:axId val="800726224"/>
-        <c:axId val="800726768"/>
+        <c:axId val="1317002736"/>
+        <c:axId val="1317003280"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="800726224"/>
+        <c:axId val="1317002736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2744,7 +2739,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="800726768"/>
+        <c:crossAx val="1317003280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2752,7 +2747,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="800726768"/>
+        <c:axId val="1317003280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2763,7 +2758,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="800726224"/>
+        <c:crossAx val="1317002736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4351,7 +4346,7 @@
   </sheetPr>
   <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -48259,7 +48254,7 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>